<commit_message>
Add arquivos aula 4
</commit_message>
<xml_diff>
--- a/data-collection/meu_arquivo.xlsx
+++ b/data-collection/meu_arquivo.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28502"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wittmann/projects/br-data-science/data-collection/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,8 +44,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +108,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -141,12 +159,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -173,14 +191,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -207,6 +226,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -382,92 +402,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>221</v>
       </c>
       <c r="B2">
-        <v>221</v>
+        <v>956</v>
       </c>
       <c r="C2">
-        <v>956</v>
+        <v>796</v>
       </c>
       <c r="D2">
-        <v>796</v>
-      </c>
-      <c r="E2">
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>1</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>879</v>
       </c>
       <c r="B3">
-        <v>879</v>
+        <v>696</v>
       </c>
       <c r="C3">
-        <v>696</v>
+        <v>875</v>
       </c>
       <c r="D3">
-        <v>875</v>
-      </c>
-      <c r="E3">
         <v>617</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>2</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>725</v>
       </c>
       <c r="B4">
-        <v>725</v>
+        <v>303</v>
       </c>
       <c r="C4">
-        <v>303</v>
+        <v>363</v>
       </c>
       <c r="D4">
-        <v>363</v>
-      </c>
-      <c r="E4">
         <v>780</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>3</v>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>538</v>
       </c>
       <c r="B5">
-        <v>538</v>
+        <v>840</v>
       </c>
       <c r="C5">
-        <v>840</v>
+        <v>247</v>
       </c>
       <c r="D5">
-        <v>247</v>
-      </c>
-      <c r="E5">
         <v>178</v>
       </c>
     </row>

</xml_diff>